<commit_message>
added template for .Renviron file
</commit_message>
<xml_diff>
--- a/codebook_data.xlsx
+++ b/codebook_data.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="116">
   <si>
     <t xml:space="preserve">Variable name</t>
   </si>
@@ -119,73 +119,97 @@
     <t xml:space="preserve">-99</t>
   </si>
   <si>
+    <t xml:space="preserve">ranking_question_ranking_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dataframe_name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Data Source Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CHAPTER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TITLE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ranking Order</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Multiple choice question</t>
+  </si>
+  <si>
+    <t xml:space="preserve">zwei</t>
+  </si>
+  <si>
+    <t xml:space="preserve">eins</t>
+  </si>
+  <si>
+    <t xml:space="preserve">drei</t>
+  </si>
+  <si>
+    <t xml:space="preserve">vier</t>
+  </si>
+  <si>
+    <t xml:space="preserve">two</t>
+  </si>
+  <si>
+    <t xml:space="preserve">one</t>
+  </si>
+  <si>
+    <t xml:space="preserve">three</t>
+  </si>
+  <si>
+    <t xml:space="preserve">four</t>
+  </si>
+  <si>
+    <t xml:space="preserve">not in panel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">unit nonresponse</t>
+  </si>
+  <si>
+    <t xml:space="preserve">missing by m.o.p.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">missing by technical error</t>
+  </si>
+  <si>
+    <t xml:space="preserve">missing by design</t>
+  </si>
+  <si>
+    <t xml:space="preserve">not reached</t>
+  </si>
+  <si>
+    <t xml:space="preserve">missing by filter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nonvalid answer in survey (e.g. ambigious)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">item nonresponse</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ranking_question_ranking_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ranking_question_ranking_3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ranking_question_ranking_4</t>
+  </si>
+  <si>
     <t xml:space="preserve">w1_MC_frage</t>
   </si>
   <si>
-    <t xml:space="preserve">dataframe_name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Data Source Name</t>
-  </si>
-  <si>
     <t xml:space="preserve">MC</t>
   </si>
   <si>
-    <t xml:space="preserve">CHAPTER</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TITLE</t>
-  </si>
-  <si>
     <t xml:space="preserve">MultipleChoice Frage</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Multiple choice question</t>
-  </si>
-  <si>
-    <t xml:space="preserve">zwei</t>
-  </si>
-  <si>
-    <t xml:space="preserve">eins</t>
-  </si>
-  <si>
-    <t xml:space="preserve">drei</t>
-  </si>
-  <si>
-    <t xml:space="preserve">two</t>
-  </si>
-  <si>
-    <t xml:space="preserve">one</t>
-  </si>
-  <si>
-    <t xml:space="preserve">three</t>
-  </si>
-  <si>
-    <t xml:space="preserve">not in panel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">unit nonresponse</t>
-  </si>
-  <si>
-    <t xml:space="preserve">missing by m.o.p.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">missing by technical error</t>
-  </si>
-  <si>
-    <t xml:space="preserve">missing by design</t>
-  </si>
-  <si>
-    <t xml:space="preserve">not reached</t>
-  </si>
-  <si>
-    <t xml:space="preserve">missing by filter</t>
-  </si>
-  <si>
-    <t xml:space="preserve">nonvalid answer in survey (e.g. ambigious)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">item nonresponse</t>
   </si>
   <si>
     <t xml:space="preserve">MC_frage_multiplex1</t>
@@ -815,51 +839,55 @@
       <c r="R2" t="s">
         <v>45</v>
       </c>
-      <c r="S2"/>
+      <c r="S2" t="s">
+        <v>46</v>
+      </c>
       <c r="T2"/>
       <c r="U2"/>
       <c r="V2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="W2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="X2" t="s">
-        <v>48</v>
-      </c>
-      <c r="Y2"/>
+        <v>49</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>50</v>
+      </c>
       <c r="Z2"/>
       <c r="AA2" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="AB2" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="AC2" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="AD2" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="AE2" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="AF2" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="AG2" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="AH2" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="AI2" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="B3"/>
       <c r="C3" t="s">
@@ -881,64 +909,72 @@
       <c r="I3"/>
       <c r="J3"/>
       <c r="K3" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="L3" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="M3"/>
       <c r="N3"/>
-      <c r="O3" t="s">
-        <v>59</v>
-      </c>
+      <c r="O3"/>
       <c r="P3" t="s">
-        <v>60</v>
-      </c>
-      <c r="Q3"/>
-      <c r="R3"/>
-      <c r="S3"/>
+        <v>43</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>44</v>
+      </c>
+      <c r="R3" t="s">
+        <v>45</v>
+      </c>
+      <c r="S3" t="s">
+        <v>46</v>
+      </c>
       <c r="T3"/>
-      <c r="U3" t="s">
-        <v>61</v>
-      </c>
+      <c r="U3"/>
       <c r="V3" t="s">
-        <v>62</v>
-      </c>
-      <c r="W3"/>
-      <c r="X3"/>
-      <c r="Y3"/>
+        <v>47</v>
+      </c>
+      <c r="W3" t="s">
+        <v>48</v>
+      </c>
+      <c r="X3" t="s">
+        <v>49</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>50</v>
+      </c>
       <c r="Z3"/>
       <c r="AA3" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="AB3" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="AC3" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="AD3" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="AE3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="AF3" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="AG3" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="AH3" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="AI3" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B4"/>
       <c r="C4" t="s">
@@ -960,64 +996,72 @@
       <c r="I4"/>
       <c r="J4"/>
       <c r="K4" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="L4" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="M4"/>
       <c r="N4"/>
-      <c r="O4" t="s">
-        <v>59</v>
-      </c>
+      <c r="O4"/>
       <c r="P4" t="s">
-        <v>60</v>
-      </c>
-      <c r="Q4"/>
-      <c r="R4"/>
-      <c r="S4"/>
+        <v>43</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>44</v>
+      </c>
+      <c r="R4" t="s">
+        <v>45</v>
+      </c>
+      <c r="S4" t="s">
+        <v>46</v>
+      </c>
       <c r="T4"/>
-      <c r="U4" t="s">
-        <v>61</v>
-      </c>
+      <c r="U4"/>
       <c r="V4" t="s">
-        <v>62</v>
-      </c>
-      <c r="W4"/>
-      <c r="X4"/>
-      <c r="Y4"/>
+        <v>47</v>
+      </c>
+      <c r="W4" t="s">
+        <v>48</v>
+      </c>
+      <c r="X4" t="s">
+        <v>49</v>
+      </c>
+      <c r="Y4" t="s">
+        <v>50</v>
+      </c>
       <c r="Z4"/>
       <c r="AA4" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="AB4" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="AC4" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="AD4" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="AE4" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="AF4" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="AG4" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="AH4" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="AI4" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B5"/>
       <c r="C5" t="s">
@@ -1039,64 +1083,72 @@
       <c r="I5"/>
       <c r="J5"/>
       <c r="K5" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="L5" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="M5"/>
       <c r="N5"/>
-      <c r="O5" t="s">
-        <v>59</v>
-      </c>
+      <c r="O5"/>
       <c r="P5" t="s">
-        <v>60</v>
-      </c>
-      <c r="Q5"/>
-      <c r="R5"/>
-      <c r="S5"/>
+        <v>43</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>44</v>
+      </c>
+      <c r="R5" t="s">
+        <v>45</v>
+      </c>
+      <c r="S5" t="s">
+        <v>46</v>
+      </c>
       <c r="T5"/>
-      <c r="U5" t="s">
-        <v>61</v>
-      </c>
+      <c r="U5"/>
       <c r="V5" t="s">
-        <v>62</v>
-      </c>
-      <c r="W5"/>
-      <c r="X5"/>
-      <c r="Y5"/>
+        <v>47</v>
+      </c>
+      <c r="W5" t="s">
+        <v>48</v>
+      </c>
+      <c r="X5" t="s">
+        <v>49</v>
+      </c>
+      <c r="Y5" t="s">
+        <v>50</v>
+      </c>
       <c r="Z5"/>
       <c r="AA5" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="AB5" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="AC5" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="AD5" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="AE5" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="AF5" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="AG5" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="AH5" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="AI5" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B6"/>
       <c r="C6" t="s">
@@ -1106,7 +1158,7 @@
         <v>37</v>
       </c>
       <c r="E6" t="s">
-        <v>38</v>
+        <v>64</v>
       </c>
       <c r="F6" t="s">
         <v>39</v>
@@ -1118,64 +1170,68 @@
       <c r="I6"/>
       <c r="J6"/>
       <c r="K6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="L6" t="s">
-        <v>67</v>
+        <v>42</v>
       </c>
       <c r="M6"/>
       <c r="N6"/>
-      <c r="O6" t="s">
-        <v>68</v>
-      </c>
+      <c r="O6"/>
       <c r="P6" t="s">
-        <v>69</v>
-      </c>
-      <c r="Q6"/>
-      <c r="R6"/>
+        <v>43</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>44</v>
+      </c>
+      <c r="R6" t="s">
+        <v>45</v>
+      </c>
       <c r="S6"/>
       <c r="T6"/>
-      <c r="U6" t="s">
+      <c r="U6"/>
+      <c r="V6" t="s">
         <v>47</v>
       </c>
-      <c r="V6" t="s">
-        <v>46</v>
-      </c>
-      <c r="W6"/>
-      <c r="X6"/>
+      <c r="W6" t="s">
+        <v>48</v>
+      </c>
+      <c r="X6" t="s">
+        <v>49</v>
+      </c>
       <c r="Y6"/>
       <c r="Z6"/>
       <c r="AA6" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="AB6" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="AC6" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="AD6" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="AE6" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="AF6" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="AG6" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="AH6" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="AI6" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="B7"/>
       <c r="C7" t="s">
@@ -1185,7 +1241,7 @@
         <v>37</v>
       </c>
       <c r="E7" t="s">
-        <v>38</v>
+        <v>64</v>
       </c>
       <c r="F7" t="s">
         <v>39</v>
@@ -1197,66 +1253,64 @@
       <c r="I7"/>
       <c r="J7"/>
       <c r="K7" t="s">
-        <v>66</v>
+        <v>44</v>
       </c>
       <c r="L7" t="s">
-        <v>67</v>
+        <v>48</v>
       </c>
       <c r="M7"/>
       <c r="N7"/>
       <c r="O7" t="s">
+        <v>67</v>
+      </c>
+      <c r="P7" t="s">
         <v>68</v>
-      </c>
-      <c r="P7" t="s">
-        <v>69</v>
       </c>
       <c r="Q7"/>
       <c r="R7"/>
       <c r="S7"/>
-      <c r="T7" t="s">
-        <v>71</v>
-      </c>
+      <c r="T7"/>
       <c r="U7" t="s">
-        <v>47</v>
+        <v>69</v>
       </c>
       <c r="V7" t="s">
-        <v>46</v>
+        <v>70</v>
       </c>
       <c r="W7"/>
       <c r="X7"/>
       <c r="Y7"/>
       <c r="Z7"/>
       <c r="AA7" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="AB7" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="AC7" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="AD7" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="AE7" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="AF7" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="AG7" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="AH7" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="AI7" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B8"/>
       <c r="C8" t="s">
@@ -1266,7 +1320,7 @@
         <v>37</v>
       </c>
       <c r="E8" t="s">
-        <v>38</v>
+        <v>64</v>
       </c>
       <c r="F8" t="s">
         <v>39</v>
@@ -1278,72 +1332,64 @@
       <c r="I8"/>
       <c r="J8"/>
       <c r="K8" t="s">
-        <v>73</v>
+        <v>43</v>
       </c>
       <c r="L8" t="s">
-        <v>74</v>
+        <v>47</v>
       </c>
       <c r="M8"/>
       <c r="N8"/>
-      <c r="O8"/>
+      <c r="O8" t="s">
+        <v>67</v>
+      </c>
       <c r="P8" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q8" t="s">
-        <v>43</v>
-      </c>
-      <c r="R8" t="s">
-        <v>45</v>
-      </c>
-      <c r="S8" t="s">
-        <v>75</v>
-      </c>
+        <v>68</v>
+      </c>
+      <c r="Q8"/>
+      <c r="R8"/>
+      <c r="S8"/>
       <c r="T8"/>
-      <c r="U8"/>
+      <c r="U8" t="s">
+        <v>69</v>
+      </c>
       <c r="V8" t="s">
-        <v>47</v>
-      </c>
-      <c r="W8" t="s">
-        <v>46</v>
-      </c>
-      <c r="X8" t="s">
-        <v>48</v>
-      </c>
-      <c r="Y8" t="s">
-        <v>76</v>
-      </c>
+        <v>70</v>
+      </c>
+      <c r="W8"/>
+      <c r="X8"/>
+      <c r="Y8"/>
       <c r="Z8"/>
       <c r="AA8" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="AB8" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="AC8" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="AD8" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="AE8" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="AF8" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="AG8" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="AH8" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="AI8" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="B9"/>
       <c r="C9" t="s">
@@ -1353,7 +1399,7 @@
         <v>37</v>
       </c>
       <c r="E9" t="s">
-        <v>38</v>
+        <v>64</v>
       </c>
       <c r="F9" t="s">
         <v>39</v>
@@ -1365,56 +1411,64 @@
       <c r="I9"/>
       <c r="J9"/>
       <c r="K9" t="s">
-        <v>73</v>
+        <v>45</v>
       </c>
       <c r="L9" t="s">
-        <v>74</v>
+        <v>49</v>
       </c>
       <c r="M9"/>
       <c r="N9"/>
-      <c r="O9"/>
-      <c r="P9"/>
+      <c r="O9" t="s">
+        <v>67</v>
+      </c>
+      <c r="P9" t="s">
+        <v>68</v>
+      </c>
       <c r="Q9"/>
       <c r="R9"/>
       <c r="S9"/>
       <c r="T9"/>
-      <c r="U9"/>
-      <c r="V9"/>
+      <c r="U9" t="s">
+        <v>69</v>
+      </c>
+      <c r="V9" t="s">
+        <v>70</v>
+      </c>
       <c r="W9"/>
       <c r="X9"/>
       <c r="Y9"/>
       <c r="Z9"/>
       <c r="AA9" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="AB9" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="AC9" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="AD9" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="AE9" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="AF9" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="AG9" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="AH9" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="AI9" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B10"/>
       <c r="C10" t="s">
@@ -1424,7 +1478,7 @@
         <v>37</v>
       </c>
       <c r="E10" t="s">
-        <v>78</v>
+        <v>64</v>
       </c>
       <c r="F10" t="s">
         <v>39</v>
@@ -1436,56 +1490,64 @@
       <c r="I10"/>
       <c r="J10"/>
       <c r="K10" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="L10" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="M10"/>
       <c r="N10"/>
-      <c r="O10"/>
-      <c r="P10"/>
+      <c r="O10" t="s">
+        <v>76</v>
+      </c>
+      <c r="P10" t="s">
+        <v>77</v>
+      </c>
       <c r="Q10"/>
       <c r="R10"/>
       <c r="S10"/>
       <c r="T10"/>
-      <c r="U10"/>
-      <c r="V10"/>
+      <c r="U10" t="s">
+        <v>48</v>
+      </c>
+      <c r="V10" t="s">
+        <v>47</v>
+      </c>
       <c r="W10"/>
       <c r="X10"/>
       <c r="Y10"/>
       <c r="Z10"/>
       <c r="AA10" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="AB10" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="AC10" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="AD10" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="AE10" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="AF10" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="AG10" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="AH10" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="AI10" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B11"/>
       <c r="C11" t="s">
@@ -1495,7 +1557,7 @@
         <v>37</v>
       </c>
       <c r="E11" t="s">
-        <v>78</v>
+        <v>64</v>
       </c>
       <c r="F11" t="s">
         <v>39</v>
@@ -1507,56 +1569,66 @@
       <c r="I11"/>
       <c r="J11"/>
       <c r="K11" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="L11" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="M11"/>
       <c r="N11"/>
-      <c r="O11"/>
-      <c r="P11"/>
+      <c r="O11" t="s">
+        <v>76</v>
+      </c>
+      <c r="P11" t="s">
+        <v>77</v>
+      </c>
       <c r="Q11"/>
       <c r="R11"/>
       <c r="S11"/>
-      <c r="T11"/>
-      <c r="U11"/>
-      <c r="V11"/>
+      <c r="T11" t="s">
+        <v>79</v>
+      </c>
+      <c r="U11" t="s">
+        <v>48</v>
+      </c>
+      <c r="V11" t="s">
+        <v>47</v>
+      </c>
       <c r="W11"/>
       <c r="X11"/>
       <c r="Y11"/>
       <c r="Z11"/>
       <c r="AA11" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="AB11" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="AC11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="AD11" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="AE11" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="AF11" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="AG11" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="AH11" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="AI11" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="B12"/>
       <c r="C12" t="s">
@@ -1566,7 +1638,7 @@
         <v>37</v>
       </c>
       <c r="E12" t="s">
-        <v>85</v>
+        <v>64</v>
       </c>
       <c r="F12" t="s">
         <v>39</v>
@@ -1578,68 +1650,72 @@
       <c r="I12"/>
       <c r="J12"/>
       <c r="K12" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="L12" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="M12"/>
       <c r="N12"/>
       <c r="O12"/>
       <c r="P12" t="s">
-        <v>88</v>
+        <v>44</v>
       </c>
       <c r="Q12" t="s">
-        <v>89</v>
+        <v>43</v>
       </c>
       <c r="R12" t="s">
-        <v>90</v>
-      </c>
-      <c r="S12"/>
+        <v>45</v>
+      </c>
+      <c r="S12" t="s">
+        <v>83</v>
+      </c>
       <c r="T12"/>
       <c r="U12"/>
       <c r="V12" t="s">
-        <v>91</v>
+        <v>48</v>
       </c>
       <c r="W12" t="s">
-        <v>92</v>
+        <v>47</v>
       </c>
       <c r="X12" t="s">
-        <v>93</v>
-      </c>
-      <c r="Y12"/>
+        <v>49</v>
+      </c>
+      <c r="Y12" t="s">
+        <v>84</v>
+      </c>
       <c r="Z12"/>
       <c r="AA12" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="AB12" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="AC12" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="AD12" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="AE12" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="AF12" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="AG12" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="AH12" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="AI12" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="B13"/>
       <c r="C13" t="s">
@@ -1649,7 +1725,7 @@
         <v>37</v>
       </c>
       <c r="E13" t="s">
-        <v>85</v>
+        <v>64</v>
       </c>
       <c r="F13" t="s">
         <v>39</v>
@@ -1661,68 +1737,56 @@
       <c r="I13"/>
       <c r="J13"/>
       <c r="K13" t="s">
-        <v>43</v>
+        <v>81</v>
       </c>
       <c r="L13" t="s">
-        <v>46</v>
+        <v>82</v>
       </c>
       <c r="M13"/>
       <c r="N13"/>
       <c r="O13"/>
-      <c r="P13" t="s">
-        <v>88</v>
-      </c>
-      <c r="Q13" t="s">
-        <v>89</v>
-      </c>
-      <c r="R13" t="s">
-        <v>90</v>
-      </c>
+      <c r="P13"/>
+      <c r="Q13"/>
+      <c r="R13"/>
       <c r="S13"/>
       <c r="T13"/>
       <c r="U13"/>
-      <c r="V13" t="s">
-        <v>91</v>
-      </c>
-      <c r="W13" t="s">
-        <v>92</v>
-      </c>
-      <c r="X13" t="s">
-        <v>93</v>
-      </c>
+      <c r="V13"/>
+      <c r="W13"/>
+      <c r="X13"/>
       <c r="Y13"/>
       <c r="Z13"/>
       <c r="AA13" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="AB13" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="AC13" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="AD13" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="AE13" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="AF13" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="AG13" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="AH13" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="AI13" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>95</v>
+        <v>83</v>
       </c>
       <c r="B14"/>
       <c r="C14" t="s">
@@ -1732,7 +1796,7 @@
         <v>37</v>
       </c>
       <c r="E14" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="F14" t="s">
         <v>39</v>
@@ -1744,68 +1808,56 @@
       <c r="I14"/>
       <c r="J14"/>
       <c r="K14" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="L14" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="M14"/>
       <c r="N14"/>
       <c r="O14"/>
-      <c r="P14" t="s">
-        <v>88</v>
-      </c>
-      <c r="Q14" t="s">
-        <v>89</v>
-      </c>
-      <c r="R14" t="s">
-        <v>90</v>
-      </c>
+      <c r="P14"/>
+      <c r="Q14"/>
+      <c r="R14"/>
       <c r="S14"/>
       <c r="T14"/>
       <c r="U14"/>
-      <c r="V14" t="s">
-        <v>91</v>
-      </c>
-      <c r="W14" t="s">
-        <v>92</v>
-      </c>
-      <c r="X14" t="s">
-        <v>93</v>
-      </c>
+      <c r="V14"/>
+      <c r="W14"/>
+      <c r="X14"/>
       <c r="Y14"/>
       <c r="Z14"/>
       <c r="AA14" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="AB14" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="AC14" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="AD14" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="AE14" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="AF14" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="AG14" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="AH14" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="AI14" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
       <c r="B15"/>
       <c r="C15" t="s">
@@ -1815,7 +1867,7 @@
         <v>37</v>
       </c>
       <c r="E15" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="F15" t="s">
         <v>39</v>
@@ -1827,68 +1879,56 @@
       <c r="I15"/>
       <c r="J15"/>
       <c r="K15" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="L15" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="M15"/>
       <c r="N15"/>
       <c r="O15"/>
-      <c r="P15" t="s">
-        <v>88</v>
-      </c>
-      <c r="Q15" t="s">
-        <v>89</v>
-      </c>
-      <c r="R15" t="s">
-        <v>90</v>
-      </c>
+      <c r="P15"/>
+      <c r="Q15"/>
+      <c r="R15"/>
       <c r="S15"/>
       <c r="T15"/>
       <c r="U15"/>
-      <c r="V15" t="s">
-        <v>91</v>
-      </c>
-      <c r="W15" t="s">
-        <v>92</v>
-      </c>
-      <c r="X15" t="s">
-        <v>93</v>
-      </c>
+      <c r="V15"/>
+      <c r="W15"/>
+      <c r="X15"/>
       <c r="Y15"/>
       <c r="Z15"/>
       <c r="AA15" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="AB15" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="AC15" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="AD15" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="AE15" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="AF15" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="AG15" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="AH15" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="AI15" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="B16"/>
       <c r="C16" t="s">
@@ -1898,7 +1938,7 @@
         <v>37</v>
       </c>
       <c r="E16" t="s">
-        <v>85</v>
+        <v>93</v>
       </c>
       <c r="F16" t="s">
         <v>39</v>
@@ -1910,68 +1950,68 @@
       <c r="I16"/>
       <c r="J16"/>
       <c r="K16" t="s">
-        <v>43</v>
+        <v>94</v>
       </c>
       <c r="L16" t="s">
-        <v>46</v>
+        <v>95</v>
       </c>
       <c r="M16"/>
       <c r="N16"/>
       <c r="O16"/>
       <c r="P16" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
       <c r="Q16" t="s">
-        <v>89</v>
+        <v>97</v>
       </c>
       <c r="R16" t="s">
-        <v>90</v>
+        <v>98</v>
       </c>
       <c r="S16"/>
       <c r="T16"/>
       <c r="U16"/>
       <c r="V16" t="s">
-        <v>91</v>
+        <v>99</v>
       </c>
       <c r="W16" t="s">
-        <v>92</v>
+        <v>100</v>
       </c>
       <c r="X16" t="s">
-        <v>93</v>
+        <v>101</v>
       </c>
       <c r="Y16"/>
       <c r="Z16"/>
       <c r="AA16" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="AB16" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="AC16" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="AD16" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="AE16" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="AF16" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="AG16" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="AH16" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="AI16" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="B17"/>
       <c r="C17" t="s">
@@ -1981,7 +2021,7 @@
         <v>37</v>
       </c>
       <c r="E17" t="s">
-        <v>85</v>
+        <v>93</v>
       </c>
       <c r="F17" t="s">
         <v>39</v>
@@ -1993,68 +2033,68 @@
       <c r="I17"/>
       <c r="J17"/>
       <c r="K17" t="s">
-        <v>96</v>
+        <v>43</v>
       </c>
       <c r="L17" t="s">
-        <v>97</v>
+        <v>47</v>
       </c>
       <c r="M17"/>
       <c r="N17"/>
       <c r="O17"/>
       <c r="P17" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
       <c r="Q17" t="s">
-        <v>89</v>
+        <v>97</v>
       </c>
       <c r="R17" t="s">
-        <v>90</v>
+        <v>98</v>
       </c>
       <c r="S17"/>
       <c r="T17"/>
       <c r="U17"/>
       <c r="V17" t="s">
-        <v>91</v>
+        <v>99</v>
       </c>
       <c r="W17" t="s">
-        <v>92</v>
+        <v>100</v>
       </c>
       <c r="X17" t="s">
-        <v>93</v>
+        <v>101</v>
       </c>
       <c r="Y17"/>
       <c r="Z17"/>
       <c r="AA17" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="AB17" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="AC17" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="AD17" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="AE17" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="AF17" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="AG17" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="AH17" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="AI17" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="B18"/>
       <c r="C18" t="s">
@@ -2064,7 +2104,7 @@
         <v>37</v>
       </c>
       <c r="E18" t="s">
-        <v>85</v>
+        <v>93</v>
       </c>
       <c r="F18" t="s">
         <v>39</v>
@@ -2076,68 +2116,68 @@
       <c r="I18"/>
       <c r="J18"/>
       <c r="K18" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="L18" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="M18"/>
       <c r="N18"/>
       <c r="O18"/>
       <c r="P18" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
       <c r="Q18" t="s">
-        <v>89</v>
+        <v>97</v>
       </c>
       <c r="R18" t="s">
-        <v>90</v>
+        <v>98</v>
       </c>
       <c r="S18"/>
       <c r="T18"/>
       <c r="U18"/>
       <c r="V18" t="s">
-        <v>91</v>
+        <v>99</v>
       </c>
       <c r="W18" t="s">
-        <v>92</v>
+        <v>100</v>
       </c>
       <c r="X18" t="s">
-        <v>93</v>
+        <v>101</v>
       </c>
       <c r="Y18"/>
       <c r="Z18"/>
       <c r="AA18" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="AB18" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="AC18" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="AD18" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="AE18" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="AF18" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="AG18" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="AH18" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="AI18" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="B19"/>
       <c r="C19" t="s">
@@ -2147,7 +2187,7 @@
         <v>37</v>
       </c>
       <c r="E19" t="s">
-        <v>85</v>
+        <v>93</v>
       </c>
       <c r="F19" t="s">
         <v>39</v>
@@ -2159,56 +2199,68 @@
       <c r="I19"/>
       <c r="J19"/>
       <c r="K19" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="L19" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="M19"/>
       <c r="N19"/>
       <c r="O19"/>
-      <c r="P19"/>
-      <c r="Q19"/>
-      <c r="R19"/>
+      <c r="P19" t="s">
+        <v>96</v>
+      </c>
+      <c r="Q19" t="s">
+        <v>97</v>
+      </c>
+      <c r="R19" t="s">
+        <v>98</v>
+      </c>
       <c r="S19"/>
       <c r="T19"/>
       <c r="U19"/>
-      <c r="V19"/>
-      <c r="W19"/>
-      <c r="X19"/>
+      <c r="V19" t="s">
+        <v>99</v>
+      </c>
+      <c r="W19" t="s">
+        <v>100</v>
+      </c>
+      <c r="X19" t="s">
+        <v>101</v>
+      </c>
       <c r="Y19"/>
       <c r="Z19"/>
       <c r="AA19" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="AB19" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="AC19" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="AD19" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="AE19" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="AF19" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="AG19" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="AH19" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="AI19" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="B20"/>
       <c r="C20" t="s">
@@ -2218,7 +2270,7 @@
         <v>37</v>
       </c>
       <c r="E20" t="s">
-        <v>38</v>
+        <v>93</v>
       </c>
       <c r="F20" t="s">
         <v>39</v>
@@ -2230,59 +2282,379 @@
       <c r="I20"/>
       <c r="J20"/>
       <c r="K20" t="s">
-        <v>106</v>
+        <v>43</v>
       </c>
       <c r="L20" t="s">
-        <v>107</v>
+        <v>47</v>
       </c>
       <c r="M20"/>
       <c r="N20"/>
       <c r="O20"/>
       <c r="P20" t="s">
-        <v>44</v>
+        <v>96</v>
       </c>
       <c r="Q20" t="s">
-        <v>43</v>
-      </c>
-      <c r="R20"/>
+        <v>97</v>
+      </c>
+      <c r="R20" t="s">
+        <v>98</v>
+      </c>
       <c r="S20"/>
       <c r="T20"/>
       <c r="U20"/>
       <c r="V20" t="s">
-        <v>47</v>
+        <v>99</v>
       </c>
       <c r="W20" t="s">
-        <v>46</v>
-      </c>
-      <c r="X20"/>
+        <v>100</v>
+      </c>
+      <c r="X20" t="s">
+        <v>101</v>
+      </c>
       <c r="Y20"/>
       <c r="Z20"/>
       <c r="AA20" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="AB20" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="AC20" t="s">
+        <v>53</v>
+      </c>
+      <c r="AD20" t="s">
+        <v>54</v>
+      </c>
+      <c r="AE20" t="s">
+        <v>55</v>
+      </c>
+      <c r="AF20" t="s">
+        <v>56</v>
+      </c>
+      <c r="AG20" t="s">
+        <v>57</v>
+      </c>
+      <c r="AH20" t="s">
+        <v>58</v>
+      </c>
+      <c r="AI20" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="s">
+        <v>108</v>
+      </c>
+      <c r="B21"/>
+      <c r="C21" t="s">
+        <v>36</v>
+      </c>
+      <c r="D21" t="s">
+        <v>37</v>
+      </c>
+      <c r="E21" t="s">
+        <v>93</v>
+      </c>
+      <c r="F21" t="s">
+        <v>39</v>
+      </c>
+      <c r="G21" t="s">
+        <v>40</v>
+      </c>
+      <c r="H21"/>
+      <c r="I21"/>
+      <c r="J21"/>
+      <c r="K21" t="s">
+        <v>104</v>
+      </c>
+      <c r="L21" t="s">
+        <v>105</v>
+      </c>
+      <c r="M21"/>
+      <c r="N21"/>
+      <c r="O21"/>
+      <c r="P21" t="s">
+        <v>96</v>
+      </c>
+      <c r="Q21" t="s">
+        <v>97</v>
+      </c>
+      <c r="R21" t="s">
+        <v>98</v>
+      </c>
+      <c r="S21"/>
+      <c r="T21"/>
+      <c r="U21"/>
+      <c r="V21" t="s">
+        <v>99</v>
+      </c>
+      <c r="W21" t="s">
+        <v>100</v>
+      </c>
+      <c r="X21" t="s">
+        <v>101</v>
+      </c>
+      <c r="Y21"/>
+      <c r="Z21"/>
+      <c r="AA21" t="s">
         <v>51</v>
       </c>
-      <c r="AD20" t="s">
+      <c r="AB21" t="s">
         <v>52</v>
       </c>
-      <c r="AE20" t="s">
+      <c r="AC21" t="s">
         <v>53</v>
       </c>
-      <c r="AF20" t="s">
+      <c r="AD21" t="s">
         <v>54</v>
       </c>
-      <c r="AG20" t="s">
+      <c r="AE21" t="s">
         <v>55</v>
       </c>
-      <c r="AH20" t="s">
+      <c r="AF21" t="s">
         <v>56</v>
       </c>
-      <c r="AI20" t="s">
+      <c r="AG21" t="s">
         <v>57</v>
+      </c>
+      <c r="AH21" t="s">
+        <v>58</v>
+      </c>
+      <c r="AI21" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="s">
+        <v>109</v>
+      </c>
+      <c r="B22"/>
+      <c r="C22" t="s">
+        <v>36</v>
+      </c>
+      <c r="D22" t="s">
+        <v>37</v>
+      </c>
+      <c r="E22" t="s">
+        <v>93</v>
+      </c>
+      <c r="F22" t="s">
+        <v>39</v>
+      </c>
+      <c r="G22" t="s">
+        <v>40</v>
+      </c>
+      <c r="H22"/>
+      <c r="I22"/>
+      <c r="J22"/>
+      <c r="K22" t="s">
+        <v>110</v>
+      </c>
+      <c r="L22" t="s">
+        <v>111</v>
+      </c>
+      <c r="M22"/>
+      <c r="N22"/>
+      <c r="O22"/>
+      <c r="P22" t="s">
+        <v>96</v>
+      </c>
+      <c r="Q22" t="s">
+        <v>97</v>
+      </c>
+      <c r="R22" t="s">
+        <v>98</v>
+      </c>
+      <c r="S22"/>
+      <c r="T22"/>
+      <c r="U22"/>
+      <c r="V22" t="s">
+        <v>99</v>
+      </c>
+      <c r="W22" t="s">
+        <v>100</v>
+      </c>
+      <c r="X22" t="s">
+        <v>101</v>
+      </c>
+      <c r="Y22"/>
+      <c r="Z22"/>
+      <c r="AA22" t="s">
+        <v>51</v>
+      </c>
+      <c r="AB22" t="s">
+        <v>52</v>
+      </c>
+      <c r="AC22" t="s">
+        <v>53</v>
+      </c>
+      <c r="AD22" t="s">
+        <v>54</v>
+      </c>
+      <c r="AE22" t="s">
+        <v>55</v>
+      </c>
+      <c r="AF22" t="s">
+        <v>56</v>
+      </c>
+      <c r="AG22" t="s">
+        <v>57</v>
+      </c>
+      <c r="AH22" t="s">
+        <v>58</v>
+      </c>
+      <c r="AI22" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="s">
+        <v>112</v>
+      </c>
+      <c r="B23"/>
+      <c r="C23" t="s">
+        <v>36</v>
+      </c>
+      <c r="D23" t="s">
+        <v>37</v>
+      </c>
+      <c r="E23" t="s">
+        <v>93</v>
+      </c>
+      <c r="F23" t="s">
+        <v>39</v>
+      </c>
+      <c r="G23" t="s">
+        <v>40</v>
+      </c>
+      <c r="H23"/>
+      <c r="I23"/>
+      <c r="J23"/>
+      <c r="K23" t="s">
+        <v>110</v>
+      </c>
+      <c r="L23" t="s">
+        <v>111</v>
+      </c>
+      <c r="M23"/>
+      <c r="N23"/>
+      <c r="O23"/>
+      <c r="P23"/>
+      <c r="Q23"/>
+      <c r="R23"/>
+      <c r="S23"/>
+      <c r="T23"/>
+      <c r="U23"/>
+      <c r="V23"/>
+      <c r="W23"/>
+      <c r="X23"/>
+      <c r="Y23"/>
+      <c r="Z23"/>
+      <c r="AA23" t="s">
+        <v>51</v>
+      </c>
+      <c r="AB23" t="s">
+        <v>52</v>
+      </c>
+      <c r="AC23" t="s">
+        <v>53</v>
+      </c>
+      <c r="AD23" t="s">
+        <v>54</v>
+      </c>
+      <c r="AE23" t="s">
+        <v>55</v>
+      </c>
+      <c r="AF23" t="s">
+        <v>56</v>
+      </c>
+      <c r="AG23" t="s">
+        <v>57</v>
+      </c>
+      <c r="AH23" t="s">
+        <v>58</v>
+      </c>
+      <c r="AI23" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="s">
+        <v>113</v>
+      </c>
+      <c r="B24"/>
+      <c r="C24" t="s">
+        <v>36</v>
+      </c>
+      <c r="D24" t="s">
+        <v>37</v>
+      </c>
+      <c r="E24" t="s">
+        <v>64</v>
+      </c>
+      <c r="F24" t="s">
+        <v>39</v>
+      </c>
+      <c r="G24" t="s">
+        <v>40</v>
+      </c>
+      <c r="H24"/>
+      <c r="I24"/>
+      <c r="J24"/>
+      <c r="K24" t="s">
+        <v>114</v>
+      </c>
+      <c r="L24" t="s">
+        <v>115</v>
+      </c>
+      <c r="M24"/>
+      <c r="N24"/>
+      <c r="O24"/>
+      <c r="P24" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q24" t="s">
+        <v>43</v>
+      </c>
+      <c r="R24"/>
+      <c r="S24"/>
+      <c r="T24"/>
+      <c r="U24"/>
+      <c r="V24" t="s">
+        <v>48</v>
+      </c>
+      <c r="W24" t="s">
+        <v>47</v>
+      </c>
+      <c r="X24"/>
+      <c r="Y24"/>
+      <c r="Z24"/>
+      <c r="AA24" t="s">
+        <v>51</v>
+      </c>
+      <c r="AB24" t="s">
+        <v>52</v>
+      </c>
+      <c r="AC24" t="s">
+        <v>53</v>
+      </c>
+      <c r="AD24" t="s">
+        <v>54</v>
+      </c>
+      <c r="AE24" t="s">
+        <v>55</v>
+      </c>
+      <c r="AF24" t="s">
+        <v>56</v>
+      </c>
+      <c r="AG24" t="s">
+        <v>57</v>
+      </c>
+      <c r="AH24" t="s">
+        <v>58</v>
+      </c>
+      <c r="AI24" t="s">
+        <v>59</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
missing codes on one page only with reference on every page
</commit_message>
<xml_diff>
--- a/codebook_data.xlsx
+++ b/codebook_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lukas\polybox - Lukas Walker (lukas.walker@gess.ethz.ch)@polybox.ethz.ch\Qualtrics\temp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E8DA5C4-FACE-4860-9ACE-8F972566E234}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6F8AA6C-E4E1-4DC5-B012-EA7ECDE8B7FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="57480" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="205">
   <si>
     <t>Variable name</t>
   </si>
@@ -632,6 +632,9 @@
   </si>
   <si>
     <t>No</t>
+  </si>
+  <si>
+    <t>ইন্টারভিউ যে নিচ্ছে</t>
   </si>
 </sst>
 </file>
@@ -967,8 +970,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:DY6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E35" sqref="E35"/>
+    <sheetView tabSelected="1" topLeftCell="BQ1" workbookViewId="0">
+      <selection activeCell="CK10" sqref="CK10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.9453125" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1385,7 +1388,7 @@
         <v>135</v>
       </c>
       <c r="L2" t="s">
-        <v>136</v>
+        <v>204</v>
       </c>
       <c r="P2" t="s">
         <v>137</v>
@@ -1515,6 +1518,12 @@
       </c>
       <c r="CJ2" t="s">
         <v>179</v>
+      </c>
+      <c r="CK2" t="s">
+        <v>157</v>
+      </c>
+      <c r="CL2" t="s">
+        <v>158</v>
       </c>
       <c r="CM2" t="s">
         <v>180</v>

</xml_diff>